<commit_message>
Removed unneeded data files
</commit_message>
<xml_diff>
--- a/data/AllData.xlsx
+++ b/data/AllData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanschaefer/Documents/SMU/2022Spring/CS3353/Projects/Project2/Program2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C506D8-D2BC-A94E-B189-234D784262E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A90AE33-E4AF-144A-9438-BCB5284BEDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="8" xr2:uid="{0351E3D1-8E73-2641-852B-06D6734494C5}"/>
+    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="7" xr2:uid="{0351E3D1-8E73-2641-852B-06D6734494C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ryan1" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,8 @@
     <sheet name="Wes2" sheetId="6" r:id="rId6"/>
     <sheet name="Wes3" sheetId="7" r:id="rId7"/>
     <sheet name="WesMean" sheetId="8" r:id="rId8"/>
-    <sheet name="Combined" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="18">
   <si>
     <t xml:space="preserve"> var_type</t>
   </si>
@@ -13299,8 +13298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D59C28-F948-7042-BC7E-813739BE4F18}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15437,2148 +15436,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DBE446-20FC-C940-8C0D-8E75523290F0}">
-  <dimension ref="A1:I61"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>500000</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <f>AVERAGE(RyanMean!D2,WesMean!D2)</f>
-        <v>928.59249999999997</v>
-      </c>
-      <c r="E2">
-        <f>AVERAGE(RyanMean!E2,WesMean!E2)</f>
-        <v>0.20632699999999998</v>
-      </c>
-      <c r="F2">
-        <f>AVERAGE(RyanMean!F2,WesMean!F2)</f>
-        <v>2.6146383333333336</v>
-      </c>
-      <c r="G2">
-        <f>AVERAGE(RyanMean!G2,WesMean!G2)</f>
-        <v>0.35297100000000003</v>
-      </c>
-      <c r="H2">
-        <f>AVERAGE(RyanMean!H2,WesMean!H2)</f>
-        <v>0.84389200000000009</v>
-      </c>
-      <c r="I2">
-        <f>AVERAGE(RyanMean!I2,WesMean!I2)</f>
-        <v>0.94704266666666659</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>1000000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <f>AVERAGE(RyanMean!D3,WesMean!D3)</f>
-        <v>3794.0600000000004</v>
-      </c>
-      <c r="E3">
-        <f>AVERAGE(RyanMean!E3,WesMean!E3)</f>
-        <v>0.38262316666666668</v>
-      </c>
-      <c r="F3">
-        <f>AVERAGE(RyanMean!F3,WesMean!F3)</f>
-        <v>5.2244299999999999</v>
-      </c>
-      <c r="G3">
-        <f>AVERAGE(RyanMean!G3,WesMean!G3)</f>
-        <v>0.77607366666666666</v>
-      </c>
-      <c r="H3">
-        <f>AVERAGE(RyanMean!H3,WesMean!H3)</f>
-        <v>1.9203116666666666</v>
-      </c>
-      <c r="I3">
-        <f>AVERAGE(RyanMean!I3,WesMean!I3)</f>
-        <v>2.0126766666666667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>100000</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <f>AVERAGE(RyanMean!D4,WesMean!D4)</f>
-        <v>37.818300000000001</v>
-      </c>
-      <c r="E4">
-        <f>AVERAGE(RyanMean!E4,WesMean!E4)</f>
-        <v>3.3999599999999998E-2</v>
-      </c>
-      <c r="F4">
-        <f>AVERAGE(RyanMean!F4,WesMean!F4)</f>
-        <v>0.51216583333333343</v>
-      </c>
-      <c r="G4">
-        <f>AVERAGE(RyanMean!G4,WesMean!G4)</f>
-        <v>5.6593233333333333E-2</v>
-      </c>
-      <c r="H4">
-        <f>AVERAGE(RyanMean!H4,WesMean!H4)</f>
-        <v>0.16745383333333333</v>
-      </c>
-      <c r="I4">
-        <f>AVERAGE(RyanMean!I4,WesMean!I4)</f>
-        <v>0.18426066666666668</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>10000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <f>AVERAGE(RyanMean!D5,WesMean!D5)</f>
-        <v>0.39220300000000002</v>
-      </c>
-      <c r="E5">
-        <f>AVERAGE(RyanMean!E5,WesMean!E5)</f>
-        <v>3.0156583333333332E-3</v>
-      </c>
-      <c r="F5">
-        <f>AVERAGE(RyanMean!F5,WesMean!F5)</f>
-        <v>4.9989033333333335E-2</v>
-      </c>
-      <c r="G5">
-        <f>AVERAGE(RyanMean!G5,WesMean!G5)</f>
-        <v>3.5379016666666667E-3</v>
-      </c>
-      <c r="H5">
-        <f>AVERAGE(RyanMean!H5,WesMean!H5)</f>
-        <v>1.360155E-2</v>
-      </c>
-      <c r="I5">
-        <f>AVERAGE(RyanMean!I5,WesMean!I5)</f>
-        <v>1.5257669999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>50000</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <f>AVERAGE(RyanMean!D6,WesMean!D6)</f>
-        <v>8.8080500000000002E-4</v>
-      </c>
-      <c r="E6">
-        <f>AVERAGE(RyanMean!E6,WesMean!E6)</f>
-        <v>1.376902E-2</v>
-      </c>
-      <c r="F6">
-        <f>AVERAGE(RyanMean!F6,WesMean!F6)</f>
-        <v>0.25437033333333336</v>
-      </c>
-      <c r="G6">
-        <f>AVERAGE(RyanMean!G6,WesMean!G6)</f>
-        <v>6.8510099999999994E-3</v>
-      </c>
-      <c r="H6">
-        <f>AVERAGE(RyanMean!H6,WesMean!H6)</f>
-        <v>7.0738550000000011E-2</v>
-      </c>
-      <c r="I6">
-        <f>AVERAGE(RyanMean!I6,WesMean!I6)</f>
-        <v>6.7643983333333338E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>50000</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <f>AVERAGE(RyanMean!D7,WesMean!D7)</f>
-        <v>9.5058900000000008</v>
-      </c>
-      <c r="E7">
-        <f>AVERAGE(RyanMean!E7,WesMean!E7)</f>
-        <v>1.6747399999999999E-2</v>
-      </c>
-      <c r="F7">
-        <f>AVERAGE(RyanMean!F7,WesMean!F7)</f>
-        <v>0.24884149999999999</v>
-      </c>
-      <c r="G7">
-        <f>AVERAGE(RyanMean!G7,WesMean!G7)</f>
-        <v>2.3602949999999998E-2</v>
-      </c>
-      <c r="H7">
-        <f>AVERAGE(RyanMean!H7,WesMean!H7)</f>
-        <v>7.5824083333333334E-2</v>
-      </c>
-      <c r="I7">
-        <f>AVERAGE(RyanMean!I7,WesMean!I7)</f>
-        <v>8.2080166666666676E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>5000</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <f>AVERAGE(RyanMean!D8,WesMean!D8)</f>
-        <v>9.7554050000000003E-2</v>
-      </c>
-      <c r="E8">
-        <f>AVERAGE(RyanMean!E8,WesMean!E8)</f>
-        <v>1.4794999999999999E-3</v>
-      </c>
-      <c r="F8">
-        <f>AVERAGE(RyanMean!F8,WesMean!F8)</f>
-        <v>2.3019899999999996E-2</v>
-      </c>
-      <c r="G8">
-        <f>AVERAGE(RyanMean!G8,WesMean!G8)</f>
-        <v>1.568615E-3</v>
-      </c>
-      <c r="H8">
-        <f>AVERAGE(RyanMean!H8,WesMean!H8)</f>
-        <v>5.9624699999999992E-3</v>
-      </c>
-      <c r="I8">
-        <f>AVERAGE(RyanMean!I8,WesMean!I8)</f>
-        <v>6.3464133333333336E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>500000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9">
-        <f>AVERAGE(RyanMean!D9,WesMean!D9)</f>
-        <v>8.6029799999999997E-3</v>
-      </c>
-      <c r="E9">
-        <f>AVERAGE(RyanMean!E9,WesMean!E9)</f>
-        <v>0.12612871666666667</v>
-      </c>
-      <c r="F9">
-        <f>AVERAGE(RyanMean!F9,WesMean!F9)</f>
-        <v>2.6839683333333335</v>
-      </c>
-      <c r="G9">
-        <f>AVERAGE(RyanMean!G9,WesMean!G9)</f>
-        <v>9.3804216666666662E-2</v>
-      </c>
-      <c r="H9">
-        <f>AVERAGE(RyanMean!H9,WesMean!H9)</f>
-        <v>0.94733233333333344</v>
-      </c>
-      <c r="I9">
-        <f>AVERAGE(RyanMean!I9,WesMean!I9)</f>
-        <v>0.91318583333333336</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>500000</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10">
-        <f>AVERAGE(RyanMean!D10,WesMean!D10)</f>
-        <v>152.6105</v>
-      </c>
-      <c r="E10">
-        <f>AVERAGE(RyanMean!E10,WesMean!E10)</f>
-        <v>0.16170033333333333</v>
-      </c>
-      <c r="F10">
-        <f>AVERAGE(RyanMean!F10,WesMean!F10)</f>
-        <v>2.7571699999999995</v>
-      </c>
-      <c r="G10">
-        <f>AVERAGE(RyanMean!G10,WesMean!G10)</f>
-        <v>0.183444</v>
-      </c>
-      <c r="H10">
-        <f>AVERAGE(RyanMean!H10,WesMean!H10)</f>
-        <v>0.9264443333333332</v>
-      </c>
-      <c r="I10">
-        <f>AVERAGE(RyanMean!I10,WesMean!I10)</f>
-        <v>0.94644066666666671</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>10000</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11">
-        <f>AVERAGE(RyanMean!D11,WesMean!D11)</f>
-        <v>6.1462050000000004E-2</v>
-      </c>
-      <c r="E11">
-        <f>AVERAGE(RyanMean!E11,WesMean!E11)</f>
-        <v>2.6381099999999999E-3</v>
-      </c>
-      <c r="F11">
-        <f>AVERAGE(RyanMean!F11,WesMean!F11)</f>
-        <v>5.1022683333333332E-2</v>
-      </c>
-      <c r="G11">
-        <f>AVERAGE(RyanMean!G11,WesMean!G11)</f>
-        <v>2.1301683333333331E-3</v>
-      </c>
-      <c r="H11">
-        <f>AVERAGE(RyanMean!H11,WesMean!H11)</f>
-        <v>1.4277321666666665E-2</v>
-      </c>
-      <c r="I11">
-        <f>AVERAGE(RyanMean!I11,WesMean!I11)</f>
-        <v>1.4156651666666666E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>1000000</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <f>AVERAGE(RyanMean!D12,WesMean!D12)</f>
-        <v>3801.0699999999997</v>
-      </c>
-      <c r="E12">
-        <f>AVERAGE(RyanMean!E12,WesMean!E12)</f>
-        <v>0.41100816666666662</v>
-      </c>
-      <c r="F12">
-        <f>AVERAGE(RyanMean!F12,WesMean!F12)</f>
-        <v>5.6368749999999999</v>
-      </c>
-      <c r="G12">
-        <f>AVERAGE(RyanMean!G12,WesMean!G12)</f>
-        <v>0.81254266666666664</v>
-      </c>
-      <c r="H12">
-        <f>AVERAGE(RyanMean!H12,WesMean!H12)</f>
-        <v>1.9554</v>
-      </c>
-      <c r="I12">
-        <f>AVERAGE(RyanMean!I12,WesMean!I12)</f>
-        <v>2.1300149999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>1000000</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13">
-        <f>AVERAGE(RyanMean!D13,WesMean!D13)</f>
-        <v>3821.29</v>
-      </c>
-      <c r="E13">
-        <f>AVERAGE(RyanMean!E13,WesMean!E13)</f>
-        <v>0.41495683333333333</v>
-      </c>
-      <c r="F13">
-        <f>AVERAGE(RyanMean!F13,WesMean!F13)</f>
-        <v>5.5454749999999997</v>
-      </c>
-      <c r="G13">
-        <f>AVERAGE(RyanMean!G13,WesMean!G13)</f>
-        <v>0.79851033333333321</v>
-      </c>
-      <c r="H13">
-        <f>AVERAGE(RyanMean!H13,WesMean!H13)</f>
-        <v>1.9299249999999999</v>
-      </c>
-      <c r="I13">
-        <f>AVERAGE(RyanMean!I13,WesMean!I13)</f>
-        <v>2.0347116666666669</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14">
-        <v>50000</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14">
-        <f>AVERAGE(RyanMean!D14,WesMean!D14)</f>
-        <v>9.5889349999999993</v>
-      </c>
-      <c r="E14">
-        <f>AVERAGE(RyanMean!E14,WesMean!E14)</f>
-        <v>1.6368799999999999E-2</v>
-      </c>
-      <c r="F14">
-        <f>AVERAGE(RyanMean!F14,WesMean!F14)</f>
-        <v>0.24949866666666665</v>
-      </c>
-      <c r="G14">
-        <f>AVERAGE(RyanMean!G14,WesMean!G14)</f>
-        <v>2.4548199999999999E-2</v>
-      </c>
-      <c r="H14">
-        <f>AVERAGE(RyanMean!H14,WesMean!H14)</f>
-        <v>7.5524066666666667E-2</v>
-      </c>
-      <c r="I14">
-        <f>AVERAGE(RyanMean!I14,WesMean!I14)</f>
-        <v>8.169966666666667E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15">
-        <v>5000</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15">
-        <f>AVERAGE(RyanMean!D15,WesMean!D15)</f>
-        <v>1.5704599999999999E-2</v>
-      </c>
-      <c r="E15">
-        <f>AVERAGE(RyanMean!E15,WesMean!E15)</f>
-        <v>1.29043E-3</v>
-      </c>
-      <c r="F15">
-        <f>AVERAGE(RyanMean!F15,WesMean!F15)</f>
-        <v>2.3205699999999999E-2</v>
-      </c>
-      <c r="G15">
-        <f>AVERAGE(RyanMean!G15,WesMean!G15)</f>
-        <v>9.320983333333335E-4</v>
-      </c>
-      <c r="H15">
-        <f>AVERAGE(RyanMean!H15,WesMean!H15)</f>
-        <v>5.896533333333333E-3</v>
-      </c>
-      <c r="I15">
-        <f>AVERAGE(RyanMean!I15,WesMean!I15)</f>
-        <v>5.8888516666666668E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16">
-        <v>5000</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16">
-        <f>AVERAGE(RyanMean!D16,WesMean!D16)</f>
-        <v>7.9939999999999997E-5</v>
-      </c>
-      <c r="E16">
-        <f>AVERAGE(RyanMean!E16,WesMean!E16)</f>
-        <v>1.0944948333333334E-3</v>
-      </c>
-      <c r="F16">
-        <f>AVERAGE(RyanMean!F16,WesMean!F16)</f>
-        <v>2.176585E-2</v>
-      </c>
-      <c r="G16">
-        <f>AVERAGE(RyanMean!G16,WesMean!G16)</f>
-        <v>5.1929950000000004E-4</v>
-      </c>
-      <c r="H16">
-        <f>AVERAGE(RyanMean!H16,WesMean!H16)</f>
-        <v>5.4894449999999999E-3</v>
-      </c>
-      <c r="I16">
-        <f>AVERAGE(RyanMean!I16,WesMean!I16)</f>
-        <v>5.4154583333333329E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17">
-        <v>100000</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17">
-        <f>AVERAGE(RyanMean!D17,WesMean!D17)</f>
-        <v>38.068449999999999</v>
-      </c>
-      <c r="E17">
-        <f>AVERAGE(RyanMean!E17,WesMean!E17)</f>
-        <v>3.402288333333333E-2</v>
-      </c>
-      <c r="F17">
-        <f>AVERAGE(RyanMean!F17,WesMean!F17)</f>
-        <v>0.50394016666666674</v>
-      </c>
-      <c r="G17">
-        <f>AVERAGE(RyanMean!G17,WesMean!G17)</f>
-        <v>5.2829050000000002E-2</v>
-      </c>
-      <c r="H17">
-        <f>AVERAGE(RyanMean!H17,WesMean!H17)</f>
-        <v>0.15646833333333332</v>
-      </c>
-      <c r="I17">
-        <f>AVERAGE(RyanMean!I17,WesMean!I17)</f>
-        <v>0.17470849999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18">
-        <v>50000</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18">
-        <f>AVERAGE(RyanMean!D18,WesMean!D18)</f>
-        <v>1.5279099999999999</v>
-      </c>
-      <c r="E18">
-        <f>AVERAGE(RyanMean!E18,WesMean!E18)</f>
-        <v>1.3458816666666668E-2</v>
-      </c>
-      <c r="F18">
-        <f>AVERAGE(RyanMean!F18,WesMean!F18)</f>
-        <v>0.23827349999999997</v>
-      </c>
-      <c r="G18">
-        <f>AVERAGE(RyanMean!G18,WesMean!G18)</f>
-        <v>1.3072938333333334E-2</v>
-      </c>
-      <c r="H18">
-        <f>AVERAGE(RyanMean!H18,WesMean!H18)</f>
-        <v>7.0147766666666667E-2</v>
-      </c>
-      <c r="I18">
-        <f>AVERAGE(RyanMean!I18,WesMean!I18)</f>
-        <v>7.0103216666666662E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19">
-        <v>10000</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19">
-        <f>AVERAGE(RyanMean!D19,WesMean!D19)</f>
-        <v>0.38781300000000002</v>
-      </c>
-      <c r="E19">
-        <f>AVERAGE(RyanMean!E19,WesMean!E19)</f>
-        <v>3.1473550000000001E-3</v>
-      </c>
-      <c r="F19">
-        <f>AVERAGE(RyanMean!F19,WesMean!F19)</f>
-        <v>4.8405233333333332E-2</v>
-      </c>
-      <c r="G19">
-        <f>AVERAGE(RyanMean!G19,WesMean!G19)</f>
-        <v>3.7878183333333332E-3</v>
-      </c>
-      <c r="H19">
-        <f>AVERAGE(RyanMean!H19,WesMean!H19)</f>
-        <v>1.3667925000000001E-2</v>
-      </c>
-      <c r="I19">
-        <f>AVERAGE(RyanMean!I19,WesMean!I19)</f>
-        <v>1.5091279999999999E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20">
-        <v>500000</v>
-      </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20">
-        <f>AVERAGE(RyanMean!D20,WesMean!D20)</f>
-        <v>951.57050000000004</v>
-      </c>
-      <c r="E20">
-        <f>AVERAGE(RyanMean!E20,WesMean!E20)</f>
-        <v>0.18800566666666665</v>
-      </c>
-      <c r="F20">
-        <f>AVERAGE(RyanMean!F20,WesMean!F20)</f>
-        <v>2.5408649999999997</v>
-      </c>
-      <c r="G20">
-        <f>AVERAGE(RyanMean!G20,WesMean!G20)</f>
-        <v>0.35276350000000001</v>
-      </c>
-      <c r="H20">
-        <f>AVERAGE(RyanMean!H20,WesMean!H20)</f>
-        <v>0.87419216666666666</v>
-      </c>
-      <c r="I20">
-        <f>AVERAGE(RyanMean!I20,WesMean!I20)</f>
-        <v>0.9471425</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21">
-        <v>500000</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21">
-        <f>AVERAGE(RyanMean!D21,WesMean!D21)</f>
-        <v>947.31600000000003</v>
-      </c>
-      <c r="E21">
-        <f>AVERAGE(RyanMean!E21,WesMean!E21)</f>
-        <v>0.18767416666666667</v>
-      </c>
-      <c r="F21">
-        <f>AVERAGE(RyanMean!F21,WesMean!F21)</f>
-        <v>2.5196450000000001</v>
-      </c>
-      <c r="G21">
-        <f>AVERAGE(RyanMean!G21,WesMean!G21)</f>
-        <v>0.34216333333333332</v>
-      </c>
-      <c r="H21">
-        <f>AVERAGE(RyanMean!H21,WesMean!H21)</f>
-        <v>0.86771033333333336</v>
-      </c>
-      <c r="I21">
-        <f>AVERAGE(RyanMean!I21,WesMean!I21)</f>
-        <v>0.9323840000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22">
-        <v>1000000</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22">
-        <f>AVERAGE(RyanMean!D22,WesMean!D22)</f>
-        <v>1.7189550000000001E-2</v>
-      </c>
-      <c r="E22">
-        <f>AVERAGE(RyanMean!E22,WesMean!E22)</f>
-        <v>0.26882099999999998</v>
-      </c>
-      <c r="F22">
-        <f>AVERAGE(RyanMean!F22,WesMean!F22)</f>
-        <v>5.0331716666666662</v>
-      </c>
-      <c r="G22">
-        <f>AVERAGE(RyanMean!G22,WesMean!G22)</f>
-        <v>0.18298049999999999</v>
-      </c>
-      <c r="H22">
-        <f>AVERAGE(RyanMean!H22,WesMean!H22)</f>
-        <v>1.7260650000000002</v>
-      </c>
-      <c r="I22">
-        <f>AVERAGE(RyanMean!I22,WesMean!I22)</f>
-        <v>1.6921983333333332</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23">
-        <v>5000</v>
-      </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23">
-        <f>AVERAGE(RyanMean!D23,WesMean!D23)</f>
-        <v>9.2812499999999992E-2</v>
-      </c>
-      <c r="E23">
-        <f>AVERAGE(RyanMean!E23,WesMean!E23)</f>
-        <v>1.4630616666666666E-3</v>
-      </c>
-      <c r="F23">
-        <f>AVERAGE(RyanMean!F23,WesMean!F23)</f>
-        <v>2.2511700000000003E-2</v>
-      </c>
-      <c r="G23">
-        <f>AVERAGE(RyanMean!G23,WesMean!G23)</f>
-        <v>1.5092433333333333E-3</v>
-      </c>
-      <c r="H23">
-        <f>AVERAGE(RyanMean!H23,WesMean!H23)</f>
-        <v>5.7810116666666654E-3</v>
-      </c>
-      <c r="I23">
-        <f>AVERAGE(RyanMean!I23,WesMean!I23)</f>
-        <v>6.3531449999999993E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <v>100000</v>
-      </c>
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24">
-        <f>AVERAGE(RyanMean!D24,WesMean!D24)</f>
-        <v>37.810499999999998</v>
-      </c>
-      <c r="E24">
-        <f>AVERAGE(RyanMean!E24,WesMean!E24)</f>
-        <v>3.3718166666666674E-2</v>
-      </c>
-      <c r="F24">
-        <f>AVERAGE(RyanMean!F24,WesMean!F24)</f>
-        <v>0.49470783333333335</v>
-      </c>
-      <c r="G24">
-        <f>AVERAGE(RyanMean!G24,WesMean!G24)</f>
-        <v>5.4667500000000008E-2</v>
-      </c>
-      <c r="H24">
-        <f>AVERAGE(RyanMean!H24,WesMean!H24)</f>
-        <v>0.15611083333333334</v>
-      </c>
-      <c r="I24">
-        <f>AVERAGE(RyanMean!I24,WesMean!I24)</f>
-        <v>0.16887433333333335</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25">
-        <v>50000</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25">
-        <f>AVERAGE(RyanMean!D25,WesMean!D25)</f>
-        <v>9.4352100000000014</v>
-      </c>
-      <c r="E25">
-        <f>AVERAGE(RyanMean!E25,WesMean!E25)</f>
-        <v>1.8693150000000002E-2</v>
-      </c>
-      <c r="F25">
-        <f>AVERAGE(RyanMean!F25,WesMean!F25)</f>
-        <v>0.24369433333333332</v>
-      </c>
-      <c r="G25">
-        <f>AVERAGE(RyanMean!G25,WesMean!G25)</f>
-        <v>2.3900866666666666E-2</v>
-      </c>
-      <c r="H25">
-        <f>AVERAGE(RyanMean!H25,WesMean!H25)</f>
-        <v>7.5078099999999995E-2</v>
-      </c>
-      <c r="I25">
-        <f>AVERAGE(RyanMean!I25,WesMean!I25)</f>
-        <v>7.8798716666666671E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26">
-        <v>10000</v>
-      </c>
-      <c r="C26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26">
-        <f>AVERAGE(RyanMean!D26,WesMean!D26)</f>
-        <v>0.38313600000000003</v>
-      </c>
-      <c r="E26">
-        <f>AVERAGE(RyanMean!E26,WesMean!E26)</f>
-        <v>3.0243066666666672E-3</v>
-      </c>
-      <c r="F26">
-        <f>AVERAGE(RyanMean!F26,WesMean!F26)</f>
-        <v>4.6134599999999998E-2</v>
-      </c>
-      <c r="G26">
-        <f>AVERAGE(RyanMean!G26,WesMean!G26)</f>
-        <v>3.5354783333333335E-3</v>
-      </c>
-      <c r="H26">
-        <f>AVERAGE(RyanMean!H26,WesMean!H26)</f>
-        <v>1.23984E-2</v>
-      </c>
-      <c r="I26">
-        <f>AVERAGE(RyanMean!I26,WesMean!I26)</f>
-        <v>1.4153950000000002E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27">
-        <v>100000</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27">
-        <f>AVERAGE(RyanMean!D27,WesMean!D27)</f>
-        <v>1.724845E-3</v>
-      </c>
-      <c r="E27">
-        <f>AVERAGE(RyanMean!E27,WesMean!E27)</f>
-        <v>2.3970783333333332E-2</v>
-      </c>
-      <c r="F27">
-        <f>AVERAGE(RyanMean!F27,WesMean!F27)</f>
-        <v>0.48152800000000001</v>
-      </c>
-      <c r="G27">
-        <f>AVERAGE(RyanMean!G27,WesMean!G27)</f>
-        <v>1.5084163333333334E-2</v>
-      </c>
-      <c r="H27">
-        <f>AVERAGE(RyanMean!H27,WesMean!H27)</f>
-        <v>0.1455255</v>
-      </c>
-      <c r="I27">
-        <f>AVERAGE(RyanMean!I27,WesMean!I27)</f>
-        <v>0.14433566666666667</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28">
-        <v>100000</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28">
-        <f>AVERAGE(RyanMean!D28,WesMean!D28)</f>
-        <v>6.0814450000000004</v>
-      </c>
-      <c r="E28">
-        <f>AVERAGE(RyanMean!E28,WesMean!E28)</f>
-        <v>2.7807483333333334E-2</v>
-      </c>
-      <c r="F28">
-        <f>AVERAGE(RyanMean!F28,WesMean!F28)</f>
-        <v>0.48339016666666668</v>
-      </c>
-      <c r="G28">
-        <f>AVERAGE(RyanMean!G28,WesMean!G28)</f>
-        <v>2.9143466666666666E-2</v>
-      </c>
-      <c r="H28">
-        <f>AVERAGE(RyanMean!H28,WesMean!H28)</f>
-        <v>0.15361116666666666</v>
-      </c>
-      <c r="I28">
-        <f>AVERAGE(RyanMean!I28,WesMean!I28)</f>
-        <v>0.14961666666666668</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29">
-        <v>10000</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29">
-        <f>AVERAGE(RyanMean!D29,WesMean!D29)</f>
-        <v>1.741495E-4</v>
-      </c>
-      <c r="E29">
-        <f>AVERAGE(RyanMean!E29,WesMean!E29)</f>
-        <v>2.2710600000000001E-3</v>
-      </c>
-      <c r="F29">
-        <f>AVERAGE(RyanMean!F29,WesMean!F29)</f>
-        <v>4.4526133333333329E-2</v>
-      </c>
-      <c r="G29">
-        <f>AVERAGE(RyanMean!G29,WesMean!G29)</f>
-        <v>1.1643966666666666E-3</v>
-      </c>
-      <c r="H29">
-        <f>AVERAGE(RyanMean!H29,WesMean!H29)</f>
-        <v>1.2083586666666667E-2</v>
-      </c>
-      <c r="I29">
-        <f>AVERAGE(RyanMean!I29,WesMean!I29)</f>
-        <v>1.1516255E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30">
-        <v>5000</v>
-      </c>
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30">
-        <f>AVERAGE(RyanMean!D30,WesMean!D30)</f>
-        <v>9.8438350000000008E-2</v>
-      </c>
-      <c r="E30">
-        <f>AVERAGE(RyanMean!E30,WesMean!E30)</f>
-        <v>1.4706133333333333E-3</v>
-      </c>
-      <c r="F30">
-        <f>AVERAGE(RyanMean!F30,WesMean!F30)</f>
-        <v>2.2610000000000002E-2</v>
-      </c>
-      <c r="G30">
-        <f>AVERAGE(RyanMean!G30,WesMean!G30)</f>
-        <v>1.6441883333333336E-3</v>
-      </c>
-      <c r="H30">
-        <f>AVERAGE(RyanMean!H30,WesMean!H30)</f>
-        <v>6.4008533333333329E-3</v>
-      </c>
-      <c r="I30">
-        <f>AVERAGE(RyanMean!I30,WesMean!I30)</f>
-        <v>7.1442266666666664E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31">
-        <v>1000000</v>
-      </c>
-      <c r="C31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31">
-        <f>AVERAGE(RyanMean!D31,WesMean!D31)</f>
-        <v>605.79550000000006</v>
-      </c>
-      <c r="E31">
-        <f>AVERAGE(RyanMean!E31,WesMean!E31)</f>
-        <v>0.32909750000000004</v>
-      </c>
-      <c r="F31">
-        <f>AVERAGE(RyanMean!F31,WesMean!F31)</f>
-        <v>5.2613450000000004</v>
-      </c>
-      <c r="G31">
-        <f>AVERAGE(RyanMean!G31,WesMean!G31)</f>
-        <v>0.38122050000000002</v>
-      </c>
-      <c r="H31">
-        <f>AVERAGE(RyanMean!H31,WesMean!H31)</f>
-        <v>1.8150900000000001</v>
-      </c>
-      <c r="I31">
-        <f>AVERAGE(RyanMean!I31,WesMean!I31)</f>
-        <v>1.8297316666666668</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32">
-        <v>50000</v>
-      </c>
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32">
-        <f>AVERAGE(RyanMean!D32,WesMean!D32)</f>
-        <v>7.0715450000000003E-3</v>
-      </c>
-      <c r="E32">
-        <f>AVERAGE(RyanMean!E32,WesMean!E32)</f>
-        <v>0.10259890000000001</v>
-      </c>
-      <c r="F32">
-        <f>AVERAGE(RyanMean!F32,WesMean!F32)</f>
-        <v>0.35941649999999997</v>
-      </c>
-      <c r="G32">
-        <f>AVERAGE(RyanMean!G32,WesMean!G32)</f>
-        <v>7.7971766666666664E-2</v>
-      </c>
-      <c r="H32">
-        <f>AVERAGE(RyanMean!H32,WesMean!H32)</f>
-        <v>0.19673516666666668</v>
-      </c>
-      <c r="I32">
-        <f>AVERAGE(RyanMean!I32,WesMean!I32)</f>
-        <v>0.17745166666666667</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33">
-        <v>500000</v>
-      </c>
-      <c r="C33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33">
-        <f>AVERAGE(RyanMean!D33,WesMean!D33)</f>
-        <v>7677.6100000000006</v>
-      </c>
-      <c r="E33">
-        <f>AVERAGE(RyanMean!E33,WesMean!E33)</f>
-        <v>1.3006198333333334</v>
-      </c>
-      <c r="F33">
-        <f>AVERAGE(RyanMean!F33,WesMean!F33)</f>
-        <v>4.5776866666666667</v>
-      </c>
-      <c r="G33">
-        <f>AVERAGE(RyanMean!G33,WesMean!G33)</f>
-        <v>3.1456883333333332</v>
-      </c>
-      <c r="H33">
-        <f>AVERAGE(RyanMean!H33,WesMean!H33)</f>
-        <v>2.7084216666666672</v>
-      </c>
-      <c r="I33">
-        <f>AVERAGE(RyanMean!I33,WesMean!I33)</f>
-        <v>3.2011449999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34">
-        <v>50000</v>
-      </c>
-      <c r="C34" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34">
-        <f>AVERAGE(RyanMean!D34,WesMean!D34)</f>
-        <v>76.311099999999996</v>
-      </c>
-      <c r="E34">
-        <f>AVERAGE(RyanMean!E34,WesMean!E34)</f>
-        <v>0.10236898333333333</v>
-      </c>
-      <c r="F34">
-        <f>AVERAGE(RyanMean!F34,WesMean!F34)</f>
-        <v>0.42131016666666671</v>
-      </c>
-      <c r="G34">
-        <f>AVERAGE(RyanMean!G34,WesMean!G34)</f>
-        <v>0.2111835</v>
-      </c>
-      <c r="H34">
-        <f>AVERAGE(RyanMean!H34,WesMean!H34)</f>
-        <v>0.21972299999999997</v>
-      </c>
-      <c r="I34">
-        <f>AVERAGE(RyanMean!I34,WesMean!I34)</f>
-        <v>0.26106316666666668</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35">
-        <v>10000</v>
-      </c>
-      <c r="C35" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35">
-        <f>AVERAGE(RyanMean!D35,WesMean!D35)</f>
-        <v>3.0607850000000001</v>
-      </c>
-      <c r="E35">
-        <f>AVERAGE(RyanMean!E35,WesMean!E35)</f>
-        <v>1.7345449999999998E-2</v>
-      </c>
-      <c r="F35">
-        <f>AVERAGE(RyanMean!F35,WesMean!F35)</f>
-        <v>7.621431666666667E-2</v>
-      </c>
-      <c r="G35">
-        <f>AVERAGE(RyanMean!G35,WesMean!G35)</f>
-        <v>2.9625366666666667E-2</v>
-      </c>
-      <c r="H35">
-        <f>AVERAGE(RyanMean!H35,WesMean!H35)</f>
-        <v>3.5755483333333331E-2</v>
-      </c>
-      <c r="I35">
-        <f>AVERAGE(RyanMean!I35,WesMean!I35)</f>
-        <v>4.5282100000000006E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>15</v>
-      </c>
-      <c r="B36">
-        <v>10000</v>
-      </c>
-      <c r="C36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36">
-        <f>AVERAGE(RyanMean!D36,WesMean!D36)</f>
-        <v>1.941865</v>
-      </c>
-      <c r="E36">
-        <f>AVERAGE(RyanMean!E36,WesMean!E36)</f>
-        <v>1.7530300000000002E-2</v>
-      </c>
-      <c r="F36">
-        <f>AVERAGE(RyanMean!F36,WesMean!F36)</f>
-        <v>7.1965083333333332E-2</v>
-      </c>
-      <c r="G36">
-        <f>AVERAGE(RyanMean!G36,WesMean!G36)</f>
-        <v>3.0016499999999995E-2</v>
-      </c>
-      <c r="H36">
-        <f>AVERAGE(RyanMean!H36,WesMean!H36)</f>
-        <v>3.6678099999999998E-2</v>
-      </c>
-      <c r="I36">
-        <f>AVERAGE(RyanMean!I36,WesMean!I36)</f>
-        <v>3.6267416666666663E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37">
-        <v>100000</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37">
-        <f>AVERAGE(RyanMean!D37,WesMean!D37)</f>
-        <v>1.48179E-2</v>
-      </c>
-      <c r="E37">
-        <f>AVERAGE(RyanMean!E37,WesMean!E37)</f>
-        <v>0.20782033333333333</v>
-      </c>
-      <c r="F37">
-        <f>AVERAGE(RyanMean!F37,WesMean!F37)</f>
-        <v>0.75133783333333337</v>
-      </c>
-      <c r="G37">
-        <f>AVERAGE(RyanMean!G37,WesMean!G37)</f>
-        <v>0.17336466666666667</v>
-      </c>
-      <c r="H37">
-        <f>AVERAGE(RyanMean!H37,WesMean!H37)</f>
-        <v>0.41863250000000007</v>
-      </c>
-      <c r="I37">
-        <f>AVERAGE(RyanMean!I37,WesMean!I37)</f>
-        <v>0.3844846666666667</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38">
-        <v>5000</v>
-      </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38">
-        <f>AVERAGE(RyanMean!D38,WesMean!D38)</f>
-        <v>0.75533549999999994</v>
-      </c>
-      <c r="E38">
-        <f>AVERAGE(RyanMean!E38,WesMean!E38)</f>
-        <v>8.0536433333333324E-3</v>
-      </c>
-      <c r="F38">
-        <f>AVERAGE(RyanMean!F38,WesMean!F38)</f>
-        <v>3.603046666666667E-2</v>
-      </c>
-      <c r="G38">
-        <f>AVERAGE(RyanMean!G38,WesMean!G38)</f>
-        <v>1.2812505000000002E-2</v>
-      </c>
-      <c r="H38">
-        <f>AVERAGE(RyanMean!H38,WesMean!H38)</f>
-        <v>1.6618183333333331E-2</v>
-      </c>
-      <c r="I38">
-        <f>AVERAGE(RyanMean!I38,WesMean!I38)</f>
-        <v>2.1617066666666667E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39">
-        <v>500000</v>
-      </c>
-      <c r="C39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39">
-        <f>AVERAGE(RyanMean!D39,WesMean!D39)</f>
-        <v>4921.09</v>
-      </c>
-      <c r="E39">
-        <f>AVERAGE(RyanMean!E39,WesMean!E39)</f>
-        <v>1.2440853333333333</v>
-      </c>
-      <c r="F39">
-        <f>AVERAGE(RyanMean!F39,WesMean!F39)</f>
-        <v>4.0764883333333337</v>
-      </c>
-      <c r="G39">
-        <f>AVERAGE(RyanMean!G39,WesMean!G39)</f>
-        <v>2.7809716666666668</v>
-      </c>
-      <c r="H39">
-        <f>AVERAGE(RyanMean!H39,WesMean!H39)</f>
-        <v>2.5378499999999997</v>
-      </c>
-      <c r="I39">
-        <f>AVERAGE(RyanMean!I39,WesMean!I39)</f>
-        <v>2.5764866666666664</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>15</v>
-      </c>
-      <c r="B40">
-        <v>50000</v>
-      </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40">
-        <f>AVERAGE(RyanMean!D40,WesMean!D40)</f>
-        <v>73.894549999999995</v>
-      </c>
-      <c r="E40">
-        <f>AVERAGE(RyanMean!E40,WesMean!E40)</f>
-        <v>0.10270243333333334</v>
-      </c>
-      <c r="F40">
-        <f>AVERAGE(RyanMean!F40,WesMean!F40)</f>
-        <v>0.40604750000000001</v>
-      </c>
-      <c r="G40">
-        <f>AVERAGE(RyanMean!G40,WesMean!G40)</f>
-        <v>0.21321216666666667</v>
-      </c>
-      <c r="H40">
-        <f>AVERAGE(RyanMean!H40,WesMean!H40)</f>
-        <v>0.20833083333333335</v>
-      </c>
-      <c r="I40">
-        <f>AVERAGE(RyanMean!I40,WesMean!I40)</f>
-        <v>0.25827</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>15</v>
-      </c>
-      <c r="B41">
-        <v>500000</v>
-      </c>
-      <c r="C41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41">
-        <f>AVERAGE(RyanMean!D41,WesMean!D41)</f>
-        <v>7515.2250000000004</v>
-      </c>
-      <c r="E41">
-        <f>AVERAGE(RyanMean!E41,WesMean!E41)</f>
-        <v>1.3316466666666666</v>
-      </c>
-      <c r="F41">
-        <f>AVERAGE(RyanMean!F41,WesMean!F41)</f>
-        <v>4.4477283333333331</v>
-      </c>
-      <c r="G41">
-        <f>AVERAGE(RyanMean!G41,WesMean!G41)</f>
-        <v>3.3530283333333335</v>
-      </c>
-      <c r="H41">
-        <f>AVERAGE(RyanMean!H41,WesMean!H41)</f>
-        <v>2.691278333333333</v>
-      </c>
-      <c r="I41">
-        <f>AVERAGE(RyanMean!I41,WesMean!I41)</f>
-        <v>3.1549699999999996</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42">
-        <v>5000</v>
-      </c>
-      <c r="C42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42">
-        <f>AVERAGE(RyanMean!D42,WesMean!D42)</f>
-        <v>0.74891750000000001</v>
-      </c>
-      <c r="E42">
-        <f>AVERAGE(RyanMean!E42,WesMean!E42)</f>
-        <v>8.2846700000000009E-3</v>
-      </c>
-      <c r="F42">
-        <f>AVERAGE(RyanMean!F42,WesMean!F42)</f>
-        <v>3.6352566666666662E-2</v>
-      </c>
-      <c r="G42">
-        <f>AVERAGE(RyanMean!G42,WesMean!G42)</f>
-        <v>1.2585220000000001E-2</v>
-      </c>
-      <c r="H42">
-        <f>AVERAGE(RyanMean!H42,WesMean!H42)</f>
-        <v>1.7345616666666668E-2</v>
-      </c>
-      <c r="I42">
-        <f>AVERAGE(RyanMean!I42,WesMean!I42)</f>
-        <v>1.9759566666666666E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>15</v>
-      </c>
-      <c r="B43">
-        <v>100000</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43">
-        <f>AVERAGE(RyanMean!D43,WesMean!D43)</f>
-        <v>300.50049999999999</v>
-      </c>
-      <c r="E43">
-        <f>AVERAGE(RyanMean!E43,WesMean!E43)</f>
-        <v>0.22139566666666666</v>
-      </c>
-      <c r="F43">
-        <f>AVERAGE(RyanMean!F43,WesMean!F43)</f>
-        <v>0.84280299999999997</v>
-      </c>
-      <c r="G43">
-        <f>AVERAGE(RyanMean!G43,WesMean!G43)</f>
-        <v>0.47497966666666669</v>
-      </c>
-      <c r="H43">
-        <f>AVERAGE(RyanMean!H43,WesMean!H43)</f>
-        <v>0.45359566666666667</v>
-      </c>
-      <c r="I43">
-        <f>AVERAGE(RyanMean!I43,WesMean!I43)</f>
-        <v>0.55511583333333325</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>15</v>
-      </c>
-      <c r="B44">
-        <v>5000</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44">
-        <f>AVERAGE(RyanMean!D44,WesMean!D44)</f>
-        <v>0.75785999999999998</v>
-      </c>
-      <c r="E44">
-        <f>AVERAGE(RyanMean!E44,WesMean!E44)</f>
-        <v>8.0168983333333346E-3</v>
-      </c>
-      <c r="F44">
-        <f>AVERAGE(RyanMean!F44,WesMean!F44)</f>
-        <v>3.6103716666666667E-2</v>
-      </c>
-      <c r="G44">
-        <f>AVERAGE(RyanMean!G44,WesMean!G44)</f>
-        <v>1.3104646666666667E-2</v>
-      </c>
-      <c r="H44">
-        <f>AVERAGE(RyanMean!H44,WesMean!H44)</f>
-        <v>1.6824250000000002E-2</v>
-      </c>
-      <c r="I44">
-        <f>AVERAGE(RyanMean!I44,WesMean!I44)</f>
-        <v>1.9876750000000002E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45">
-        <v>100000</v>
-      </c>
-      <c r="C45" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45">
-        <f>AVERAGE(RyanMean!D45,WesMean!D45)</f>
-        <v>192.405</v>
-      </c>
-      <c r="E45">
-        <f>AVERAGE(RyanMean!E45,WesMean!E45)</f>
-        <v>0.21585266666666666</v>
-      </c>
-      <c r="F45">
-        <f>AVERAGE(RyanMean!F45,WesMean!F45)</f>
-        <v>0.78265899999999999</v>
-      </c>
-      <c r="G45">
-        <f>AVERAGE(RyanMean!G45,WesMean!G45)</f>
-        <v>0.45494133333333331</v>
-      </c>
-      <c r="H45">
-        <f>AVERAGE(RyanMean!H45,WesMean!H45)</f>
-        <v>0.43917250000000002</v>
-      </c>
-      <c r="I45">
-        <f>AVERAGE(RyanMean!I45,WesMean!I45)</f>
-        <v>0.45534483333333331</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>15</v>
-      </c>
-      <c r="B46">
-        <v>1000000</v>
-      </c>
-      <c r="C46" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46">
-        <f>AVERAGE(RyanMean!D46,WesMean!D46)</f>
-        <v>30541.899999999998</v>
-      </c>
-      <c r="E46">
-        <f>AVERAGE(RyanMean!E46,WesMean!E46)</f>
-        <v>2.7525483333333329</v>
-      </c>
-      <c r="F46">
-        <f>AVERAGE(RyanMean!F46,WesMean!F46)</f>
-        <v>9.2505000000000006</v>
-      </c>
-      <c r="G46">
-        <f>AVERAGE(RyanMean!G46,WesMean!G46)</f>
-        <v>7.5871533333333332</v>
-      </c>
-      <c r="H46">
-        <f>AVERAGE(RyanMean!H46,WesMean!H46)</f>
-        <v>5.6705583333333331</v>
-      </c>
-      <c r="I46">
-        <f>AVERAGE(RyanMean!I46,WesMean!I46)</f>
-        <v>6.6786266666666663</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47">
-        <v>10000</v>
-      </c>
-      <c r="C47" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47">
-        <f>AVERAGE(RyanMean!D47,WesMean!D47)</f>
-        <v>3.0380250000000002</v>
-      </c>
-      <c r="E47">
-        <f>AVERAGE(RyanMean!E47,WesMean!E47)</f>
-        <v>2.03553E-2</v>
-      </c>
-      <c r="F47">
-        <f>AVERAGE(RyanMean!F47,WesMean!F47)</f>
-        <v>7.6556700000000005E-2</v>
-      </c>
-      <c r="G47">
-        <f>AVERAGE(RyanMean!G47,WesMean!G47)</f>
-        <v>3.1396566666666667E-2</v>
-      </c>
-      <c r="H47">
-        <f>AVERAGE(RyanMean!H47,WesMean!H47)</f>
-        <v>4.3000916666666666E-2</v>
-      </c>
-      <c r="I47">
-        <f>AVERAGE(RyanMean!I47,WesMean!I47)</f>
-        <v>4.5159116666666665E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>15</v>
-      </c>
-      <c r="B48">
-        <v>1000000</v>
-      </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48">
-        <f>AVERAGE(RyanMean!D48,WesMean!D48)</f>
-        <v>31924.550000000003</v>
-      </c>
-      <c r="E48">
-        <f>AVERAGE(RyanMean!E48,WesMean!E48)</f>
-        <v>2.9536433333333338</v>
-      </c>
-      <c r="F48">
-        <f>AVERAGE(RyanMean!F48,WesMean!F48)</f>
-        <v>9.9439283333333321</v>
-      </c>
-      <c r="G48">
-        <f>AVERAGE(RyanMean!G48,WesMean!G48)</f>
-        <v>7.7543733333333336</v>
-      </c>
-      <c r="H48">
-        <f>AVERAGE(RyanMean!H48,WesMean!H48)</f>
-        <v>6.186868333333333</v>
-      </c>
-      <c r="I48">
-        <f>AVERAGE(RyanMean!I48,WesMean!I48)</f>
-        <v>7.270081666666667</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>15</v>
-      </c>
-      <c r="B49">
-        <v>1000000</v>
-      </c>
-      <c r="C49" t="s">
-        <v>12</v>
-      </c>
-      <c r="D49">
-        <f>AVERAGE(RyanMean!D49,WesMean!D49)</f>
-        <v>0.16526299999999999</v>
-      </c>
-      <c r="E49">
-        <f>AVERAGE(RyanMean!E49,WesMean!E49)</f>
-        <v>2.6931633333333336</v>
-      </c>
-      <c r="F49">
-        <f>AVERAGE(RyanMean!F49,WesMean!F49)</f>
-        <v>8.9726533333333336</v>
-      </c>
-      <c r="G49">
-        <f>AVERAGE(RyanMean!G49,WesMean!G49)</f>
-        <v>2.071555</v>
-      </c>
-      <c r="H49">
-        <f>AVERAGE(RyanMean!H49,WesMean!H49)</f>
-        <v>6.2699316666666665</v>
-      </c>
-      <c r="I49">
-        <f>AVERAGE(RyanMean!I49,WesMean!I49)</f>
-        <v>5.1117983333333328</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>15</v>
-      </c>
-      <c r="B50">
-        <v>500000</v>
-      </c>
-      <c r="C50" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50">
-        <f>AVERAGE(RyanMean!D50,WesMean!D50)</f>
-        <v>8534.84</v>
-      </c>
-      <c r="E50">
-        <f>AVERAGE(RyanMean!E50,WesMean!E50)</f>
-        <v>1.2908183333333332</v>
-      </c>
-      <c r="F50">
-        <f>AVERAGE(RyanMean!F50,WesMean!F50)</f>
-        <v>4.4560950000000004</v>
-      </c>
-      <c r="G50">
-        <f>AVERAGE(RyanMean!G50,WesMean!G50)</f>
-        <v>3.0920199999999998</v>
-      </c>
-      <c r="H50">
-        <f>AVERAGE(RyanMean!H50,WesMean!H50)</f>
-        <v>2.5991866666666663</v>
-      </c>
-      <c r="I50">
-        <f>AVERAGE(RyanMean!I50,WesMean!I50)</f>
-        <v>3.2124183333333329</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51">
-        <v>100000</v>
-      </c>
-      <c r="C51" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51">
-        <f>AVERAGE(RyanMean!D51,WesMean!D51)</f>
-        <v>304.96449999999999</v>
-      </c>
-      <c r="E51">
-        <f>AVERAGE(RyanMean!E51,WesMean!E51)</f>
-        <v>0.23016599999999998</v>
-      </c>
-      <c r="F51">
-        <f>AVERAGE(RyanMean!F51,WesMean!F51)</f>
-        <v>0.84875566666666658</v>
-      </c>
-      <c r="G51">
-        <f>AVERAGE(RyanMean!G51,WesMean!G51)</f>
-        <v>0.48878333333333335</v>
-      </c>
-      <c r="H51">
-        <f>AVERAGE(RyanMean!H51,WesMean!H51)</f>
-        <v>0.45825233333333337</v>
-      </c>
-      <c r="I51">
-        <f>AVERAGE(RyanMean!I51,WesMean!I51)</f>
-        <v>0.55623199999999995</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>15</v>
-      </c>
-      <c r="B52">
-        <v>5000</v>
-      </c>
-      <c r="C52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52">
-        <f>AVERAGE(RyanMean!D52,WesMean!D52)</f>
-        <v>0.47659150000000006</v>
-      </c>
-      <c r="E52">
-        <f>AVERAGE(RyanMean!E52,WesMean!E52)</f>
-        <v>7.9373299999999994E-3</v>
-      </c>
-      <c r="F52">
-        <f>AVERAGE(RyanMean!F52,WesMean!F52)</f>
-        <v>3.5186050000000003E-2</v>
-      </c>
-      <c r="G52">
-        <f>AVERAGE(RyanMean!G52,WesMean!G52)</f>
-        <v>1.1447624999999999E-2</v>
-      </c>
-      <c r="H52">
-        <f>AVERAGE(RyanMean!H52,WesMean!H52)</f>
-        <v>1.5932483333333334E-2</v>
-      </c>
-      <c r="I52">
-        <f>AVERAGE(RyanMean!I52,WesMean!I52)</f>
-        <v>1.6620466666666663E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>15</v>
-      </c>
-      <c r="B53">
-        <v>1000000</v>
-      </c>
-      <c r="C53" t="s">
-        <v>14</v>
-      </c>
-      <c r="D53">
-        <f>AVERAGE(RyanMean!D53,WesMean!D53)</f>
-        <v>19952.150000000001</v>
-      </c>
-      <c r="E53">
-        <f>AVERAGE(RyanMean!E53,WesMean!E53)</f>
-        <v>2.6745133333333335</v>
-      </c>
-      <c r="F53">
-        <f>AVERAGE(RyanMean!F53,WesMean!F53)</f>
-        <v>8.5216849999999997</v>
-      </c>
-      <c r="G53">
-        <f>AVERAGE(RyanMean!G53,WesMean!G53)</f>
-        <v>6.28681</v>
-      </c>
-      <c r="H53">
-        <f>AVERAGE(RyanMean!H53,WesMean!H53)</f>
-        <v>5.6090933333333339</v>
-      </c>
-      <c r="I53">
-        <f>AVERAGE(RyanMean!I53,WesMean!I53)</f>
-        <v>5.5671533333333327</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B54">
-        <v>5000</v>
-      </c>
-      <c r="C54" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54">
-        <f>AVERAGE(RyanMean!D54,WesMean!D54)</f>
-        <v>6.6322050000000002E-4</v>
-      </c>
-      <c r="E54">
-        <f>AVERAGE(RyanMean!E54,WesMean!E54)</f>
-        <v>7.4052966666666668E-3</v>
-      </c>
-      <c r="F54">
-        <f>AVERAGE(RyanMean!F54,WesMean!F54)</f>
-        <v>3.3081050000000001E-2</v>
-      </c>
-      <c r="G54">
-        <f>AVERAGE(RyanMean!G54,WesMean!G54)</f>
-        <v>6.2467216666666665E-3</v>
-      </c>
-      <c r="H54">
-        <f>AVERAGE(RyanMean!H54,WesMean!H54)</f>
-        <v>1.6007283333333334E-2</v>
-      </c>
-      <c r="I54">
-        <f>AVERAGE(RyanMean!I54,WesMean!I54)</f>
-        <v>1.3668128333333335E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>15</v>
-      </c>
-      <c r="B55">
-        <v>100000</v>
-      </c>
-      <c r="C55" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55">
-        <f>AVERAGE(RyanMean!D55,WesMean!D55)</f>
-        <v>307.04950000000002</v>
-      </c>
-      <c r="E55">
-        <f>AVERAGE(RyanMean!E55,WesMean!E55)</f>
-        <v>0.22329283333333333</v>
-      </c>
-      <c r="F55">
-        <f>AVERAGE(RyanMean!F55,WesMean!F55)</f>
-        <v>0.84737950000000017</v>
-      </c>
-      <c r="G55">
-        <f>AVERAGE(RyanMean!G55,WesMean!G55)</f>
-        <v>0.49994466666666659</v>
-      </c>
-      <c r="H55">
-        <f>AVERAGE(RyanMean!H55,WesMean!H55)</f>
-        <v>0.49036516666666663</v>
-      </c>
-      <c r="I55">
-        <f>AVERAGE(RyanMean!I55,WesMean!I55)</f>
-        <v>0.56959300000000002</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>15</v>
-      </c>
-      <c r="B56">
-        <v>10000</v>
-      </c>
-      <c r="C56" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56">
-        <f>AVERAGE(RyanMean!D56,WesMean!D56)</f>
-        <v>3.04535</v>
-      </c>
-      <c r="E56">
-        <f>AVERAGE(RyanMean!E56,WesMean!E56)</f>
-        <v>1.9640949999999997E-2</v>
-      </c>
-      <c r="F56">
-        <f>AVERAGE(RyanMean!F56,WesMean!F56)</f>
-        <v>7.9478483333333322E-2</v>
-      </c>
-      <c r="G56">
-        <f>AVERAGE(RyanMean!G56,WesMean!G56)</f>
-        <v>2.9829383333333334E-2</v>
-      </c>
-      <c r="H56">
-        <f>AVERAGE(RyanMean!H56,WesMean!H56)</f>
-        <v>3.4127299999999999E-2</v>
-      </c>
-      <c r="I56">
-        <f>AVERAGE(RyanMean!I56,WesMean!I56)</f>
-        <v>4.3808050000000001E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>15</v>
-      </c>
-      <c r="B57">
-        <v>10000</v>
-      </c>
-      <c r="C57" t="s">
-        <v>12</v>
-      </c>
-      <c r="D57">
-        <f>AVERAGE(RyanMean!D57,WesMean!D57)</f>
-        <v>1.41344E-3</v>
-      </c>
-      <c r="E57">
-        <f>AVERAGE(RyanMean!E57,WesMean!E57)</f>
-        <v>1.69576E-2</v>
-      </c>
-      <c r="F57">
-        <f>AVERAGE(RyanMean!F57,WesMean!F57)</f>
-        <v>6.7889016666666663E-2</v>
-      </c>
-      <c r="G57">
-        <f>AVERAGE(RyanMean!G57,WesMean!G57)</f>
-        <v>1.3447901666666666E-2</v>
-      </c>
-      <c r="H57">
-        <f>AVERAGE(RyanMean!H57,WesMean!H57)</f>
-        <v>3.4099066666666664E-2</v>
-      </c>
-      <c r="I57">
-        <f>AVERAGE(RyanMean!I57,WesMean!I57)</f>
-        <v>3.2859733333333335E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>15</v>
-      </c>
-      <c r="B58">
-        <v>500000</v>
-      </c>
-      <c r="C58" t="s">
-        <v>12</v>
-      </c>
-      <c r="D58">
-        <f>AVERAGE(RyanMean!D58,WesMean!D58)</f>
-        <v>7.1408050000000001E-2</v>
-      </c>
-      <c r="E58">
-        <f>AVERAGE(RyanMean!E58,WesMean!E58)</f>
-        <v>1.2305753333333334</v>
-      </c>
-      <c r="F58">
-        <f>AVERAGE(RyanMean!F58,WesMean!F58)</f>
-        <v>3.9300583333333332</v>
-      </c>
-      <c r="G58">
-        <f>AVERAGE(RyanMean!G58,WesMean!G58)</f>
-        <v>0.96368750000000003</v>
-      </c>
-      <c r="H58">
-        <f>AVERAGE(RyanMean!H58,WesMean!H58)</f>
-        <v>2.5045116666666667</v>
-      </c>
-      <c r="I58">
-        <f>AVERAGE(RyanMean!I58,WesMean!I58)</f>
-        <v>2.2347483333333331</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>15</v>
-      </c>
-      <c r="B59">
-        <v>50000</v>
-      </c>
-      <c r="C59" t="s">
-        <v>11</v>
-      </c>
-      <c r="D59">
-        <f>AVERAGE(RyanMean!D59,WesMean!D59)</f>
-        <v>76.630499999999998</v>
-      </c>
-      <c r="E59">
-        <f>AVERAGE(RyanMean!E59,WesMean!E59)</f>
-        <v>0.10607844999999999</v>
-      </c>
-      <c r="F59">
-        <f>AVERAGE(RyanMean!F59,WesMean!F59)</f>
-        <v>0.41228883333333333</v>
-      </c>
-      <c r="G59">
-        <f>AVERAGE(RyanMean!G59,WesMean!G59)</f>
-        <v>0.2138835</v>
-      </c>
-      <c r="H59">
-        <f>AVERAGE(RyanMean!H59,WesMean!H59)</f>
-        <v>0.21309899999999998</v>
-      </c>
-      <c r="I59">
-        <f>AVERAGE(RyanMean!I59,WesMean!I59)</f>
-        <v>0.2609475</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>15</v>
-      </c>
-      <c r="B60">
-        <v>50000</v>
-      </c>
-      <c r="C60" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60">
-        <f>AVERAGE(RyanMean!D60,WesMean!D60)</f>
-        <v>49.581450000000004</v>
-      </c>
-      <c r="E60">
-        <f>AVERAGE(RyanMean!E60,WesMean!E60)</f>
-        <v>0.10364705</v>
-      </c>
-      <c r="F60">
-        <f>AVERAGE(RyanMean!F60,WesMean!F60)</f>
-        <v>0.37648733333333334</v>
-      </c>
-      <c r="G60">
-        <f>AVERAGE(RyanMean!G60,WesMean!G60)</f>
-        <v>0.19994999999999999</v>
-      </c>
-      <c r="H60">
-        <f>AVERAGE(RyanMean!H60,WesMean!H60)</f>
-        <v>0.21136983333333337</v>
-      </c>
-      <c r="I60">
-        <f>AVERAGE(RyanMean!I60,WesMean!I60)</f>
-        <v>0.21379233333333331</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>15</v>
-      </c>
-      <c r="B61">
-        <v>1000000</v>
-      </c>
-      <c r="C61" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61">
-        <f>AVERAGE(RyanMean!D61,WesMean!D61)</f>
-        <v>30755.95</v>
-      </c>
-      <c r="E61">
-        <f>AVERAGE(RyanMean!E61,WesMean!E61)</f>
-        <v>2.6959233333333334</v>
-      </c>
-      <c r="F61">
-        <f>AVERAGE(RyanMean!F61,WesMean!F61)</f>
-        <v>9.2105449999999998</v>
-      </c>
-      <c r="G61">
-        <f>AVERAGE(RyanMean!G61,WesMean!G61)</f>
-        <v>7.2245033333333328</v>
-      </c>
-      <c r="H61">
-        <f>AVERAGE(RyanMean!H61,WesMean!H61)</f>
-        <v>5.739863333333334</v>
-      </c>
-      <c r="I61">
-        <f>AVERAGE(RyanMean!I61,WesMean!I61)</f>
-        <v>6.7698233333333349</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>